<commit_message>
Colores bien generalizados y cambios de color
</commit_message>
<xml_diff>
--- a/IA/filas/resultados_filas.xlsx
+++ b/IA/filas/resultados_filas.xlsx
@@ -484,55 +484,55 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>153e7965-cb50-4b3f-bd22-d57e1be8a208_fila_15.png</t>
+          <t>0479f849-3354-4b13-bc69-7b30043bd56e_fila_10.png</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Orlando Mauricio Guevara</t>
+          <t>Abraham Silva Ampre</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>274f26b8-17b1-428a-b64c-75d6da8b272a_fila_3.png</t>
+          <t>315628bb-db42-48bc-8fe3-31ea92794346_fila_1.png</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Bryan Alexander Cano</t>
+          <t>Hotep Antonio Ruiz Lezama</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>47c1c7f1-969e-4997-9b4d-18e78bf9bc49_fila_4.png</t>
+          <t>3a478992-9152-48ad-ae2c-d8a0fc05e7ba_fila_13.png</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Yadder Fernando Torres</t>
+          <t>Marlon Josue Gonzales Cano</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>545e46e4-c664-4303-b493-e2e538d974e4_fila_8.png</t>
+          <t>3c943684-5c12-4960-b9aa-75089d79a55d_fila_4.png</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>David Orlando Mena Valverde</t>
+          <t>Yadder Fernando Torres</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>651af538-51aa-41b4-aa48-a2ecd734bac6_fila_9.png</t>
+          <t>3f3a7c2f-0abc-47fc-af0b-accf90aed4d5_fila_9.png</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -544,7 +544,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>6b532376-8929-4db9-b7c9-e8bcd04e572c_fila_6.png</t>
+          <t>57df3fb7-62cb-4e4d-bce7-5ef755df64f1_fila_6.png</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -556,7 +556,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>71c4d525-122a-4d20-aaf2-63e4c9fe660d_fila_2.png</t>
+          <t>648ad02a-46de-4ec7-b602-adc46e8705eb_fila_2.png</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -568,96 +568,96 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>793ad159-67b3-42cf-a2a3-f38d96f1a745_fila_14.png</t>
+          <t>676ad72f-8b15-4c34-b497-3fcc0fdc1249_fila_7.png</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Angel Isaac Alvarez Quiñonez</t>
+          <t>Cristina Jozabed Carvajal</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>829509e5-f4dd-43ad-aae3-abf57bb0d42b_fila_10.png</t>
+          <t>89fdf458-71de-4059-b799-073878fac609_fila_14.png</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Abraham Silva Ampre</t>
+          <t>Angel Isaac Alvarez Quiñonez</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>838bbe8d-8257-44e8-813a-eae2efc0f566_fila_13.png</t>
+          <t>b41224c4-a34d-48fa-a1cc-287876b653ea_fila_8.png</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Marlon Josue Gonzales Cano</t>
+          <t>David Orlando Mena Valverde</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>984b6309-7b5c-4eb9-80da-48a6c02ed257_fila_12.png</t>
+          <t>c8324d8f-0bbc-458f-b62a-6631c96ce433_fila_5.png</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>José Danilo Suárez</t>
+          <t>Erick Espinoza</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>a2646dd9-835e-4fdf-831a-1b8d9635b51d_fila_1.png</t>
+          <t>de39c47b-8c5a-4f19-b6bf-508419360394_fila_3.png</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Hotep Antonio Ruiz Lezama</t>
+          <t>Bryan Alexander Cano</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ad93756b-17d6-48a6-8b87-713283aa985c_fila_7.png</t>
+          <t>e774e6cd-a59a-41dc-b8e5-754879731161_fila_12.png</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Cristina Jozabed Carvajal</t>
+          <t>José Danilo Suárez</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>c4166ab5-a7eb-4b98-805b-a778c436d914_fila_5.png</t>
+          <t>f16b2728-ccac-4f7a-84c0-c1333af701e8_fila_11.png</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Erick Espinoza</t>
+          <t>Eduardo Domingo Zeledon Merca</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>ffd91c8a-ab1b-4118-90d6-79c3a74053a6_fila_11.png</t>
+          <t>fe13f750-c24d-4cd3-b041-3d76d19e3c54_fila_15.png</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Eduardo Domingo Zeledon Merca</t>
+          <t>Orlando Mauricio Guevara</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
heuristicas: tamaño letra, colores.
</commit_message>
<xml_diff>
--- a/IA/filas/resultados_filas.xlsx
+++ b/IA/filas/resultados_filas.xlsx
@@ -484,180 +484,180 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>0479f849-3354-4b13-bc69-7b30043bd56e_fila_10.png</t>
+          <t>02377c58-c63b-4909-ae81-26307cbed822_fila_3.png</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Abraham Silva Ampre</t>
+          <t>Bryan Alexander Cano</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>315628bb-db42-48bc-8fe3-31ea92794346_fila_1.png</t>
+          <t>04c2c643-8418-4c59-9388-c1fe7e051078_fila_15.png</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Hotep Antonio Ruiz Lezama</t>
+          <t>Orlando Mauricio Guevara</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>3a478992-9152-48ad-ae2c-d8a0fc05e7ba_fila_13.png</t>
+          <t>301feecf-684e-4a1f-8cfc-e9df5b86810d_fila_6.png</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Marlon Josue Gonzales Cano</t>
+          <t>Ronier Jose Rivera</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>3c943684-5c12-4960-b9aa-75089d79a55d_fila_4.png</t>
+          <t>426d1ee3-4fdd-400d-91b1-bf0f1760517a_fila_11.png</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Yadder Fernando Torres</t>
+          <t>Eduardo Domingo Zeledon Merca</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>3f3a7c2f-0abc-47fc-af0b-accf90aed4d5_fila_9.png</t>
+          <t>5adf0760-4db8-4070-a8db-fa3511386cd9_fila_13.png</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Roman Alfonso Grios Boza</t>
+          <t>Marlon Josue Gonzales Cano</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>57df3fb7-62cb-4e4d-bce7-5ef755df64f1_fila_6.png</t>
+          <t>861de668-39d4-4f42-848a-3a971aede11c_fila_7.png</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Ronier Jose Rivera</t>
+          <t>Cristina Jozabed Carvajal</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>648ad02a-46de-4ec7-b602-adc46e8705eb_fila_2.png</t>
+          <t>8761e7cc-4053-4584-8484-a93f3eb8f579_fila_1.png</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Isabella Dompe Estrada</t>
+          <t>Hotep Antonio Ruiz Lezama</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>676ad72f-8b15-4c34-b497-3fcc0fdc1249_fila_7.png</t>
+          <t>92d91427-2627-495a-82fc-41c4b429288d_fila_9.png</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Cristina Jozabed Carvajal</t>
+          <t>Roman Alfonso Grios Boza</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>89fdf458-71de-4059-b799-073878fac609_fila_14.png</t>
+          <t>ac476561-3453-4971-a125-3dc3dd45b57e_fila_8.png</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Angel Isaac Alvarez Quiñonez</t>
+          <t>David Orlando Mena Valverd</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>b41224c4-a34d-48fa-a1cc-287876b653ea_fila_8.png</t>
+          <t>ba29fedb-0bbb-4116-b897-21633ceec33f_fila_12.png</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>David Orlando Mena Valverde</t>
+          <t>José Danilo Suárez</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>c8324d8f-0bbc-458f-b62a-6631c96ce433_fila_5.png</t>
+          <t>bf716bf7-4eeb-4e59-9ce7-a0a2cf5d9e07_fila_4.png</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Erick Espinoza</t>
+          <t>Yadder Fernando Torres</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>de39c47b-8c5a-4f19-b6bf-508419360394_fila_3.png</t>
+          <t>c3373abb-5514-4b69-a93c-d0d5e6b7721c_fila_14.png</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Bryan Alexander Cano</t>
+          <t>Angel Isaac Alvarez Quiñonez</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>e774e6cd-a59a-41dc-b8e5-754879731161_fila_12.png</t>
+          <t>d0821fe8-c624-4bde-bc4a-31285f86fe5f_fila_5.png</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>José Danilo Suárez</t>
+          <t>Erick Espinoza</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>f16b2728-ccac-4f7a-84c0-c1333af701e8_fila_11.png</t>
+          <t>d67424cf-7e61-4dd8-b055-56013819a37a_fila_10.png</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Eduardo Domingo Zeledon Merca</t>
+          <t>Abraham Silva Ampre</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>fe13f750-c24d-4cd3-b041-3d76d19e3c54_fila_15.png</t>
+          <t>f483cc6d-c37b-4d63-b7ed-204354164760_fila_2.png</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Orlando Mauricio Guevara</t>
+          <t>Isabella Dompe Estrada</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
edicion de la tabla funcional
</commit_message>
<xml_diff>
--- a/IA/filas/resultados_filas.xlsx
+++ b/IA/filas/resultados_filas.xlsx
@@ -484,115 +484,115 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>02377c58-c63b-4909-ae81-26307cbed822_fila_3.png</t>
+          <t>0fea9b83-0187-4b9a-a30d-7fcc468cd795_fila_8.png</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Bryan Alexander Cano</t>
+          <t>David Orlando Mena Valverd</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>04c2c643-8418-4c59-9388-c1fe7e051078_fila_15.png</t>
+          <t>25ca8875-48b9-4d6f-83a1-64c6c65b79f1_fila_13.png</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Orlando Mauricio Guevara</t>
+          <t>Marlon Josue Gonzales Cano</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>301feecf-684e-4a1f-8cfc-e9df5b86810d_fila_6.png</t>
+          <t>2d21abef-a261-4e7f-a2a7-27a463ef0506_fila_15.png</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ronier Jose Rivera</t>
+          <t>Orlando Mauricio Guevara</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>426d1ee3-4fdd-400d-91b1-bf0f1760517a_fila_11.png</t>
+          <t>5b439dc6-6e18-4fc1-af77-a153f1f91b73_fila_6.png</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Eduardo Domingo Zeledon Merca</t>
+          <t>Ronier Jose Rivera</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>5adf0760-4db8-4070-a8db-fa3511386cd9_fila_13.png</t>
+          <t>84817d56-0c2f-4152-9108-ba0206098ae6_fila_9.png</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Marlon Josue Gonzales Cano</t>
+          <t>Roman Alfonso Grios Boza</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>861de668-39d4-4f42-848a-3a971aede11c_fila_7.png</t>
+          <t>a2219dad-4ed3-4a04-8e41-3f7c3e410c44_fila_11.png</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Cristina Jozabed Carvajal</t>
+          <t>Eduardo Domingo Zeledon Merca</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>8761e7cc-4053-4584-8484-a93f3eb8f579_fila_1.png</t>
+          <t>a6c522d8-c904-4bd2-9498-dd63a5af504a_fila_5.png</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Hotep Antonio Ruiz Lezama</t>
+          <t>Erick Espinoza</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>92d91427-2627-495a-82fc-41c4b429288d_fila_9.png</t>
+          <t>ac574bc6-1ae8-46d2-95a3-2d91342d0985_fila_14.png</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Roman Alfonso Grios Boza</t>
+          <t>Angel Isaac Alvarez Quiñonez</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ac476561-3453-4971-a125-3dc3dd45b57e_fila_8.png</t>
+          <t>d00088f5-e013-47c4-a206-c36bd854fe67_fila_3.png</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>David Orlando Mena Valverd</t>
+          <t>Bryan Alexander Cano</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ba29fedb-0bbb-4116-b897-21633ceec33f_fila_12.png</t>
+          <t>d0eee7e1-571b-48c0-80dc-df11791526f7_fila_12.png</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -604,60 +604,60 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>bf716bf7-4eeb-4e59-9ce7-a0a2cf5d9e07_fila_4.png</t>
+          <t>d2a27921-1ef0-416c-b85e-a1a08eab12be_fila_1.png</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Yadder Fernando Torres</t>
+          <t>Hotep Antonio Ruiz Lezama</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>c3373abb-5514-4b69-a93c-d0d5e6b7721c_fila_14.png</t>
+          <t>d5fba4c7-5088-4065-9ae9-f668048c0c92_fila_4.png</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Angel Isaac Alvarez Quiñonez</t>
+          <t>Yadder Fernando Torres</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>d0821fe8-c624-4bde-bc4a-31285f86fe5f_fila_5.png</t>
+          <t>db3cc54e-26a2-4d73-b2be-2b3d23ca4f1c_fila_2.png</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Erick Espinoza</t>
+          <t>Isabella Dompe Estrada</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>d67424cf-7e61-4dd8-b055-56013819a37a_fila_10.png</t>
+          <t>efcde127-403b-4b2d-b9a7-c10f543c35ed_fila_7.png</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Abraham Silva Ampre</t>
+          <t>Cristina Jozabed Carvajal</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>f483cc6d-c37b-4d63-b7ed-204354164760_fila_2.png</t>
+          <t>f512c4d8-3979-45e8-8f96-3317e7d77d27_fila_10.png</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Isabella Dompe Estrada</t>
+          <t>Abraham Silva Ampre</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
codigo casi listo, salida imprevista
</commit_message>
<xml_diff>
--- a/IA/filas/resultados_filas.xlsx
+++ b/IA/filas/resultados_filas.xlsx
@@ -484,180 +484,180 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>0a1a3fd1-c322-4441-a0c7-e29104ffdc99_fila_14.png</t>
+          <t>2579a007-7ce0-45df-9b42-f43695ee8fe6_fila_4.png</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Angel Isaac Alvarez Quiñonez</t>
+          <t>Yadder Fernando Torres</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>0c1d3e51-6ffd-4922-81f2-8ef077cc702e_fila_3.png</t>
+          <t>2fa5f1fa-52da-410b-bb24-4b81feae4923_fila_9.png</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Bryan Alexander Cano</t>
+          <t>Roman Alfonso Grios Boza</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1bee14eb-b9b1-44a1-9ea7-90d8693d7074_fila_13.png</t>
+          <t>387f12a5-1bfc-4f1a-8266-e9bb5d3e65e8_fila_14.png</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Marlon Josue Gonzales Cano</t>
+          <t>Angel Isaac Alvarez Quiñonez</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>232de4ba-3758-4cc7-b3ac-7125127d96a8_fila_9.png</t>
+          <t>3900499e-472d-46ac-bfc6-94423a039dea_fila_13.png</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Roman Alfonso Grios Boza</t>
+          <t>Marlon Josue Gonzales Cano</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>353593c7-14b1-46b6-a306-bfe36bd3c7b0_fila_12.png</t>
+          <t>5fdfb4ee-51c6-4975-890d-de3fd11b4ae0_fila_5.png</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>José Danilo Suárez</t>
+          <t>Erick Espinoza</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>532c257b-c201-4f0e-8bc9-07945b8ea6ca_fila_2.png</t>
+          <t>804e69c0-37bb-4675-a506-6cec1fcb206e_fila_1.png</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Isabella Dompe Estrada</t>
+          <t>Hotep Antonio Ruiz Lezama</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>79e34696-29c7-4d9c-9d36-a9cef184a387_fila_11.png</t>
+          <t>8b1dca71-2ffd-49e8-ae06-f050609aee13_fila_2.png</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Eduardo Domingo Zeledon Merca</t>
+          <t>Isabella Dompe Estrada</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>7ecb9a3c-6d6f-4927-bdb2-c85eb9fb9757_fila_7.png</t>
+          <t>96a2ae22-6463-4021-a822-307dc50678bc_fila_10.png</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Cristina Jozabed Carvajal</t>
+          <t>Abraham Silva Ampre</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>904ace37-dc45-48fb-a46c-7d066077520e_fila_15.png</t>
+          <t>9a9c70a0-158f-4e69-8dcc-a6518bb51ba2_fila_6.png</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Orlando Mauricio Guevara</t>
+          <t>Ronier Jose Rivera</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>9654f3f0-b941-4001-bc93-b4a78162eb65_fila_6.png</t>
+          <t>9c8d2642-f51f-409f-99dd-b3d8034b8fc2_fila_8.png</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Ronier Jose Rivera</t>
+          <t>David Orlando Mena Valverd</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>a040194c-b41c-4240-b9ed-ad8993b35292_fila_10.png</t>
+          <t>a0b46958-419f-4cc6-9e71-d471a237eaf5_fila_15.png</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Abraham Silva Ampre</t>
+          <t>Orlando Mauricio Guevara</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>b3a583d3-e0bb-4bed-83ef-9a44d01e59c5_fila_4.png</t>
+          <t>c630cac0-49a2-4c52-837c-96b9495fa9ab_fila_3.png</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Yadder Fernando Torres</t>
+          <t>Bryan Alexander Cano</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>dc4bb144-cb65-4807-8b29-d9e368f15e09_fila_5.png</t>
+          <t>c9dcc57c-96d6-4867-9724-cf96190a2f89_fila_7.png</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Erick Espinoza</t>
+          <t>Cristina Jozabed Carvajal</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>e520c434-a619-4aae-9633-be0288aeecde_fila_1.png</t>
+          <t>e9016cc4-85a0-442f-9865-bda3a3086566_fila_11.png</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Hotep Antonio Ruiz Lezama</t>
+          <t>Eduardo Domingo Zeledon Merca</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>f1f076f9-917f-4989-aebe-6e6d5d9978f7_fila_8.png</t>
+          <t>e9071e59-145b-4d3b-853e-043cd79ae634_fila_12.png</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>David Orlando Mena Valverd</t>
+          <t>José Danilo Suárez</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
ultimos cambios, revisiones ISO
</commit_message>
<xml_diff>
--- a/IA/filas/resultados_filas.xlsx
+++ b/IA/filas/resultados_filas.xlsx
@@ -484,43 +484,43 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1f114c3b-8ef5-4ad4-977a-604f2d2ea29a_fila_8.png</t>
+          <t>025da00d-c7d8-4f5b-9d8b-af717f607614_fila_9.png</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>David Orlando Mena Valverd</t>
+          <t>Roman Alfonso Grios Boza</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>24aa44f6-850f-4a94-8441-95a72bef18dd_fila_9.png</t>
+          <t>1d7d3ca2-ae91-448b-a30f-af7eab2a3978_fila_15.png</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Roman Alfonso Grios Boza</t>
+          <t>Orlando Mauricio Guevara</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2d3bcfb8-81ac-4330-b883-71e58a91e857_fila_1.png</t>
+          <t>1ea081eb-fb66-47f3-89e9-c8d075c539d8_fila_7.png</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Hotep Antonio Ruiz Lezama</t>
+          <t>Cristina Jozabed Carvajal</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2daf813d-2737-499b-9ff5-ee96093fdd28_fila_2.png</t>
+          <t>3088def7-058f-48af-80af-065076c246c4_fila_2.png</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -532,7 +532,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>3a4cbddc-541f-4e1c-b2a5-6921d7aed4fe_fila_10.png</t>
+          <t>39a55e95-dcfd-45f2-aabc-e9b0290f16dd_fila_10.png</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -544,115 +544,115 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>50a405b7-ac30-4011-8d3d-3b6b4d8ea491_fila_11.png</t>
+          <t>3b6de5df-f0f9-4db5-8b6f-0e7e1a36e18d_fila_4.png</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Eduardo Domingo Zeledon Merca</t>
+          <t>Yadder Fernando Torres</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>7e2834c3-c55d-4da4-9c04-f8a2a9266291_fila_7.png</t>
+          <t>4342cc05-bbbd-4d09-a2a2-06a6308c1337_fila_13.png</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Cristina Jozabed Carvajal</t>
+          <t>Marlon Josue Gonzales Cano</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>aaf18118-de1c-481c-8f68-b9fd687ca3cd_fila_5.png</t>
+          <t>4ea9709c-9a55-4a66-8562-d88a0007d197_fila_6.png</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Erick Espinoza</t>
+          <t>Ronier Jose Rivera</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>b559c412-e1b5-40dd-84ee-1fd3e037b6a9_fila_13.png</t>
+          <t>6580d43c-5690-42f2-80f6-4d378a94affe_fila_14.png</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Marlon Josue Gonzales Cano</t>
+          <t>Angel Isaac Alvarez Quiñonez</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>d5a789b7-b0ed-4d0a-85ce-60cdd8719db8_fila_3.png</t>
+          <t>7dd4e43e-d4d2-4fee-977e-b13b6f1c0891_fila_11.png</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Bryan Alexander Cano</t>
+          <t>Eduardo Domingo Zeledon Merca</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>d72c2567-f10b-44b0-a9f7-15959cf4ec6f_fila_14.png</t>
+          <t>7e15a2d1-7b5f-454e-9c6f-d7df58f942c8_fila_3.png</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Angel Isaac Alvarez Quiñonez</t>
+          <t>Bryan Alexander Cano</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>e382aeaa-2931-4471-b5fd-e3cef151b0f6_fila_4.png</t>
+          <t>8facc7e6-bab2-46a0-a3d5-c6673c096089_fila_8.png</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Yadder Fernando Torres</t>
+          <t>David Orlando Mena Valverd</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ea708df1-7ee9-4fca-a6e2-eb810aaf809c_fila_6.png</t>
+          <t>c4c25ca5-7f6c-4c1a-a605-cc3c09be6af7_fila_5.png</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Ronier Jose Rivera</t>
+          <t>Erick Espinoza</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>ec447e1a-4103-4458-8951-9d88822cafcf_fila_15.png</t>
+          <t>ca020dc0-339a-4fee-b903-5359cade4990_fila_1.png</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Orlando Mauricio Guevara</t>
+          <t>Hotep Antonio Ruiz Lezama</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>fca86bca-901e-4069-b3aa-295f253daa86_fila_12.png</t>
+          <t>cb9afc98-07fa-433d-b7e5-573c05fb955c_fila_12.png</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">

</xml_diff>